<commit_message>
Erica makes sript for phenology ground truthing
</commit_message>
<xml_diff>
--- a/data/phenology/groundtruthing_2022/FINAL_phenocam_groundtruthing_common_garden22_copy5.xlsx
+++ b/data/phenology/groundtruthing_2022/FINAL_phenocam_groundtruthing_common_garden22_copy5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericazaja/Desktop/Github_repos.tmp/GardenHub/data/phenology/groundtruthing_2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{12D14F0D-DA7B-F741-8B7E-8900DCBD8642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D542973-8918-FA47-83AE-96993CE2F94D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="620" windowWidth="24640" windowHeight="15980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="121">
   <si>
     <t>Bed</t>
   </si>
@@ -381,6 +381,9 @@
   </si>
   <si>
     <t>P6_5_first_leaf_shed</t>
+  </si>
+  <si>
+    <t>Notes 12/08</t>
   </si>
 </sst>
 </file>
@@ -743,13 +746,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AC257"/>
+  <dimension ref="A1:AA257"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="K9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L13" sqref="L13"/>
+      <selection pane="bottomRight" activeCell="M36" sqref="M36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -763,12 +766,10 @@
     <col min="12" max="12" width="19.83203125" customWidth="1"/>
     <col min="13" max="13" width="24.6640625" customWidth="1"/>
     <col min="14" max="14" width="30.6640625" customWidth="1"/>
-    <col min="15" max="15" width="12.6640625" customWidth="1"/>
-    <col min="16" max="16" width="24.5" customWidth="1"/>
-    <col min="17" max="29" width="12.6640625" customWidth="1"/>
+    <col min="15" max="27" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -814,7 +815,9 @@
       <c r="O1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="P1" s="4"/>
+      <c r="P1" s="3" t="s">
+        <v>120</v>
+      </c>
       <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
       <c r="S1" s="4"/>
@@ -826,10 +829,8 @@
       <c r="Y1" s="4"/>
       <c r="Z1" s="4"/>
       <c r="AA1" s="4"/>
-      <c r="AB1" s="4"/>
-      <c r="AC1" s="4"/>
-    </row>
-    <row r="2" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="2" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
@@ -856,7 +857,7 @@
         <v>44743</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -883,7 +884,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -906,7 +907,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="5" t="s">
         <v>15</v>
       </c>
@@ -941,7 +942,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -966,11 +967,11 @@
       <c r="M6" t="s">
         <v>24</v>
       </c>
-      <c r="R6" s="10" t="s">
+      <c r="P6" s="10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -991,7 +992,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="5" t="s">
         <v>27</v>
       </c>
@@ -1017,7 +1018,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -1046,7 +1047,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -1076,7 +1077,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="5" t="s">
         <v>36</v>
       </c>
@@ -1099,7 +1100,7 @@
         <v>44785</v>
       </c>
     </row>
-    <row r="12" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>36</v>
       </c>
@@ -1122,7 +1123,7 @@
         <v>44785</v>
       </c>
     </row>
-    <row r="13" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -1139,7 +1140,7 @@
         <v>44745</v>
       </c>
     </row>
-    <row r="14" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="5" t="s">
         <v>40</v>
       </c>
@@ -1164,11 +1165,11 @@
       <c r="M14" t="s">
         <v>24</v>
       </c>
-      <c r="R14" s="10" t="s">
+      <c r="P14" s="10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>40</v>
       </c>
@@ -1191,7 +1192,7 @@
         <v>44785</v>
       </c>
     </row>
-    <row r="16" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>40</v>
       </c>
@@ -1213,11 +1214,11 @@
       <c r="L16" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="R16" s="10" t="s">
+      <c r="P16" s="10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="5" t="s">
         <v>44</v>
       </c>
@@ -1246,7 +1247,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>44</v>
       </c>
@@ -1269,7 +1270,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>44</v>
       </c>
@@ -1292,7 +1293,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="5" t="s">
         <v>51</v>
       </c>
@@ -1312,7 +1313,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>51</v>
       </c>
@@ -1335,7 +1336,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>51</v>
       </c>
@@ -1355,7 +1356,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="5" t="s">
         <v>56</v>
       </c>
@@ -1375,7 +1376,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>56</v>
       </c>
@@ -1395,7 +1396,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>56</v>
       </c>
@@ -1412,7 +1413,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="5" t="s">
         <v>60</v>
       </c>
@@ -1434,11 +1435,11 @@
       <c r="L26" s="11">
         <v>44785</v>
       </c>
-      <c r="R26" s="10" t="s">
+      <c r="P26" s="10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>60</v>
       </c>
@@ -1458,7 +1459,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="28" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>60</v>
       </c>
@@ -1481,7 +1482,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="29" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="5" t="s">
         <v>66</v>
       </c>
@@ -1510,7 +1511,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="30" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>66</v>
       </c>
@@ -1542,7 +1543,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="31" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>66</v>
       </c>
@@ -1562,7 +1563,7 @@
         <v>44785</v>
       </c>
     </row>
-    <row r="32" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="5" t="s">
         <v>71</v>
       </c>
@@ -1585,7 +1586,7 @@
         <v>44765</v>
       </c>
     </row>
-    <row r="33" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>71</v>
       </c>
@@ -1608,7 +1609,7 @@
         <v>44785</v>
       </c>
     </row>
-    <row r="34" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>71</v>
       </c>
@@ -1631,7 +1632,7 @@
         <v>44785</v>
       </c>
     </row>
-    <row r="35" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="5" t="s">
         <v>75</v>
       </c>
@@ -1661,7 +1662,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="36" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>75</v>
       </c>
@@ -1686,11 +1687,11 @@
       <c r="M36" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="R36" s="10" t="s">
+      <c r="P36" s="10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>75</v>
       </c>
@@ -1713,7 +1714,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="38" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="5" t="s">
         <v>80</v>
       </c>
@@ -1730,7 +1731,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
         <v>80</v>
       </c>
@@ -1750,7 +1751,7 @@
         <v>44785</v>
       </c>
     </row>
-    <row r="40" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
         <v>80</v>
       </c>
@@ -1776,7 +1777,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="41" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="5" t="s">
         <v>85</v>
       </c>
@@ -1799,7 +1800,7 @@
         <v>44785</v>
       </c>
     </row>
-    <row r="42" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
         <v>85</v>
       </c>
@@ -1822,7 +1823,7 @@
         <v>44785</v>
       </c>
     </row>
-    <row r="43" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
         <v>85</v>
       </c>
@@ -1845,7 +1846,7 @@
         <v>44785</v>
       </c>
     </row>
-    <row r="44" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="5" t="s">
         <v>89</v>
       </c>
@@ -1871,7 +1872,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="45" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
         <v>89</v>
       </c>
@@ -1894,7 +1895,7 @@
         <v>44785</v>
       </c>
     </row>
-    <row r="46" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
         <v>89</v>
       </c>
@@ -1917,8 +1918,8 @@
         <v>44785</v>
       </c>
     </row>
-    <row r="47" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="48" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="47" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="48" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="49" spans="12:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="50" spans="12:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="51" spans="12:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
E adds phenology ground truthing
</commit_message>
<xml_diff>
--- a/data/phenology/groundtruthing_2022/FINAL_phenocam_groundtruthing_common_garden22_copy5.xlsx
+++ b/data/phenology/groundtruthing_2022/FINAL_phenocam_groundtruthing_common_garden22_copy5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericazaja/Desktop/Github_repos.tmp/GardenHub/data/phenology/groundtruthing_2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D542973-8918-FA47-83AE-96993CE2F94D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65EB8B22-04FA-A242-B05A-2C16F8E2F9FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="620" windowWidth="24640" windowHeight="15980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,9 +44,6 @@
     <t>A</t>
   </si>
   <si>
-    <t>KLSPE2</t>
-  </si>
-  <si>
     <t>pulchra</t>
   </si>
   <si>
@@ -56,24 +53,15 @@
     <t>B</t>
   </si>
   <si>
-    <t>KLSPE4</t>
-  </si>
-  <si>
     <t>31/07/22</t>
   </si>
   <si>
     <t>C</t>
   </si>
   <si>
-    <t>KLSPE3</t>
-  </si>
-  <si>
     <t>LB</t>
   </si>
   <si>
-    <t>KLSRE4</t>
-  </si>
-  <si>
     <t>richardsonii</t>
   </si>
   <si>
@@ -92,36 +80,21 @@
     <t>Crunchy leaves on one branch</t>
   </si>
   <si>
-    <t>H17SR4</t>
-  </si>
-  <si>
     <t>Yellow leaves from nutrient deficiency 27/06/22</t>
   </si>
   <si>
     <t>No leaves</t>
   </si>
   <si>
-    <t>KP16SR41</t>
-  </si>
-  <si>
     <t>SL</t>
   </si>
   <si>
-    <t>KP17SP5</t>
-  </si>
-  <si>
     <t>dry leaves (03/07/22)</t>
   </si>
   <si>
-    <t>H18SP15</t>
-  </si>
-  <si>
     <t>dry 10/07</t>
   </si>
   <si>
-    <t>PC17SP1</t>
-  </si>
-  <si>
     <t>rust (03/07/22)</t>
   </si>
   <si>
@@ -134,177 +107,69 @@
     <t>GD</t>
   </si>
   <si>
-    <t>H17SR9</t>
-  </si>
-  <si>
-    <t>H18SR8</t>
-  </si>
-  <si>
-    <t>K16SR37</t>
-  </si>
-  <si>
     <t>SW</t>
   </si>
   <si>
-    <t>HESR8</t>
-  </si>
-  <si>
-    <t>H15SR19</t>
-  </si>
-  <si>
-    <t>H15SR20</t>
-  </si>
-  <si>
     <t>CF</t>
   </si>
   <si>
-    <t>H15SP15</t>
-  </si>
-  <si>
     <t>Crunchy 27/06/22</t>
   </si>
   <si>
     <t>crunchy</t>
   </si>
   <si>
-    <t>H17SP9</t>
-  </si>
-  <si>
-    <t>KLSPE8</t>
-  </si>
-  <si>
     <t>female?</t>
   </si>
   <si>
     <t>JA</t>
   </si>
   <si>
-    <t>K17SA5</t>
-  </si>
-  <si>
     <t>arctica</t>
   </si>
   <si>
-    <t>KP17SA1</t>
-  </si>
-  <si>
-    <t>KP18SA4</t>
-  </si>
-  <si>
     <t>JG</t>
   </si>
   <si>
-    <t>KP18SP4</t>
-  </si>
-  <si>
-    <t>KP18SP2</t>
-  </si>
-  <si>
-    <t>KP18SP1</t>
-  </si>
-  <si>
     <t>MG</t>
   </si>
   <si>
-    <t>HESP17</t>
-  </si>
-  <si>
-    <t>KLSPE12</t>
-  </si>
-  <si>
     <t>Dry branch and leaves (03/07/22)</t>
   </si>
   <si>
-    <t>KLSPE11</t>
-  </si>
-  <si>
     <t>Crunchy dead?</t>
   </si>
   <si>
     <t>IR</t>
   </si>
   <si>
-    <t>KLSRE15</t>
-  </si>
-  <si>
     <t>catkin burst estimated (missed last time)</t>
   </si>
   <si>
-    <t>KLSRC10</t>
-  </si>
-  <si>
-    <t>KLSRE14</t>
-  </si>
-  <si>
     <t>SAB</t>
   </si>
   <si>
-    <t>H17SA15</t>
-  </si>
-  <si>
-    <t>HE16SA14</t>
-  </si>
-  <si>
-    <t>H18SA8</t>
-  </si>
-  <si>
     <t>AC</t>
   </si>
   <si>
-    <t xml:space="preserve">KLSRC13 </t>
-  </si>
-  <si>
-    <t>H15SR29</t>
-  </si>
-  <si>
     <t>No leaves (12/08/23)</t>
   </si>
   <si>
-    <t>HESR23</t>
-  </si>
-  <si>
     <t>AB</t>
   </si>
   <si>
-    <t>PC16CESP7</t>
-  </si>
-  <si>
-    <t>H17SP0</t>
-  </si>
-  <si>
-    <t>H15SP27</t>
-  </si>
-  <si>
     <t>yellow from disease</t>
   </si>
   <si>
     <t>JB</t>
   </si>
   <si>
-    <t>H17SA20</t>
-  </si>
-  <si>
-    <t>K15PSA9</t>
-  </si>
-  <si>
-    <t>H15SA12</t>
-  </si>
-  <si>
     <t>EW</t>
   </si>
   <si>
-    <t>KP18SA8</t>
-  </si>
-  <si>
     <t xml:space="preserve">Yellow leaves pics taken </t>
   </si>
   <si>
-    <t>H17sr37</t>
-  </si>
-  <si>
-    <t>H18SR27</t>
-  </si>
-  <si>
     <t>&lt;- drop down menu for previous sheet</t>
   </si>
   <si>
@@ -384,6 +249,141 @@
   </si>
   <si>
     <t>Notes 12/08</t>
+  </si>
+  <si>
+    <t>KLSpE2</t>
+  </si>
+  <si>
+    <t>KLSpE4</t>
+  </si>
+  <si>
+    <t>KLSpE3</t>
+  </si>
+  <si>
+    <t>KLSrE4</t>
+  </si>
+  <si>
+    <t>H17Sr4</t>
+  </si>
+  <si>
+    <t>KP16Sr41</t>
+  </si>
+  <si>
+    <t>KP17Sp5</t>
+  </si>
+  <si>
+    <t>H18Sp15</t>
+  </si>
+  <si>
+    <t>PC17Sp1</t>
+  </si>
+  <si>
+    <t>H17Sr9</t>
+  </si>
+  <si>
+    <t>H18Sr8</t>
+  </si>
+  <si>
+    <t>K16Sr37</t>
+  </si>
+  <si>
+    <t>HESr8</t>
+  </si>
+  <si>
+    <t>H15Sr19</t>
+  </si>
+  <si>
+    <t>H15Sr20</t>
+  </si>
+  <si>
+    <t>H15Sp15</t>
+  </si>
+  <si>
+    <t>H17Sp9</t>
+  </si>
+  <si>
+    <t>KLSpE8</t>
+  </si>
+  <si>
+    <t>K17Sa5</t>
+  </si>
+  <si>
+    <t>KP17Sa1</t>
+  </si>
+  <si>
+    <t>KP18Sa4</t>
+  </si>
+  <si>
+    <t>KP18Sp4</t>
+  </si>
+  <si>
+    <t>KP18Sp2</t>
+  </si>
+  <si>
+    <t>KP18Sp1</t>
+  </si>
+  <si>
+    <t>HESp17</t>
+  </si>
+  <si>
+    <t>KLSpE12</t>
+  </si>
+  <si>
+    <t>KLSpE11</t>
+  </si>
+  <si>
+    <t>KLSrE15</t>
+  </si>
+  <si>
+    <t>KLSrC10</t>
+  </si>
+  <si>
+    <t>KLSrE14</t>
+  </si>
+  <si>
+    <t>H17Sa15</t>
+  </si>
+  <si>
+    <t>HE16Sa14</t>
+  </si>
+  <si>
+    <t>H18Sa8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KLSrC13 </t>
+  </si>
+  <si>
+    <t>H15Sr29</t>
+  </si>
+  <si>
+    <t>HESr23</t>
+  </si>
+  <si>
+    <t>PC16CESp7</t>
+  </si>
+  <si>
+    <t>H17Sp0</t>
+  </si>
+  <si>
+    <t>H15Sp27</t>
+  </si>
+  <si>
+    <t>H17Sa20</t>
+  </si>
+  <si>
+    <t>K15PSa9</t>
+  </si>
+  <si>
+    <t>H15Sa12</t>
+  </si>
+  <si>
+    <t>KP18Sa8</t>
+  </si>
+  <si>
+    <t>H17Sr37</t>
+  </si>
+  <si>
+    <t>H18Sr27</t>
   </si>
 </sst>
 </file>
@@ -748,11 +748,11 @@
   </sheetPr>
   <dimension ref="A1:AA257"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="K9" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="234" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="E37" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M36" sqref="M36"/>
+      <selection pane="bottomRight" activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -774,37 +774,37 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>110</v>
+        <v>65</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>111</v>
+        <v>66</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>112</v>
+        <v>67</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>113</v>
+        <v>68</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>114</v>
+        <v>69</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>115</v>
+        <v>70</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>116</v>
+        <v>71</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>117</v>
+        <v>72</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>118</v>
+        <v>73</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>119</v>
+        <v>74</v>
       </c>
       <c r="M1" s="3" t="s">
         <v>2</v>
@@ -816,7 +816,7 @@
         <v>4</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>120</v>
+        <v>75</v>
       </c>
       <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
@@ -838,13 +838,13 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
       </c>
       <c r="G2" s="6">
         <v>44745</v>
@@ -862,16 +862,16 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>77</v>
       </c>
       <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
         <v>8</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
       </c>
       <c r="G3" s="6">
         <v>44745</v>
@@ -881,7 +881,7 @@
       </c>
       <c r="I3" s="7"/>
       <c r="J3" s="8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -889,13 +889,13 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>78</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F4" s="6">
         <v>44752</v>
@@ -904,24 +904,24 @@
         <v>44752</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>79</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="H5" s="9">
         <v>44732</v>
@@ -930,30 +930,30 @@
         <v>44745</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="L5" s="10" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="M5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="N5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>80</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="J6" s="6">
         <v>44745</v>
@@ -965,71 +965,71 @@
         <v>44785</v>
       </c>
       <c r="M6" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="P6" s="10" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D7" t="s">
         <v>13</v>
-      </c>
-      <c r="C7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" t="s">
-        <v>17</v>
       </c>
       <c r="J7" s="6">
         <v>44745</v>
       </c>
       <c r="K7" s="8"/>
       <c r="M7" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="5" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>82</v>
       </c>
       <c r="D8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J8" s="6">
         <v>44752</v>
       </c>
       <c r="K8" s="10" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="L8" s="6">
         <v>44765</v>
       </c>
       <c r="M8" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
       <c r="D9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J9" s="6">
         <v>44745</v>
@@ -1041,24 +1041,24 @@
         <v>44785</v>
       </c>
       <c r="M9" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="N9" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>84</v>
       </c>
       <c r="D10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J10" s="6">
         <v>44752</v>
@@ -1068,33 +1068,33 @@
         <v>44785</v>
       </c>
       <c r="M10" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="N10" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="O10" s="8" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="5" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>37</v>
+        <v>85</v>
       </c>
       <c r="D11" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="J11" s="6">
         <v>44752</v>
       </c>
       <c r="K11" s="10" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="L11" s="11">
         <v>44785</v>
@@ -1102,19 +1102,19 @@
     </row>
     <row r="12" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>86</v>
       </c>
       <c r="D12" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="J12" s="8" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="K12" s="11">
         <v>44785</v>
@@ -1125,16 +1125,16 @@
     </row>
     <row r="13" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D13" t="s">
         <v>13</v>
-      </c>
-      <c r="C13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D13" t="s">
-        <v>17</v>
       </c>
       <c r="J13" s="6">
         <v>44745</v>
@@ -1142,16 +1142,16 @@
     </row>
     <row r="14" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="5" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="B14" t="s">
         <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>41</v>
+        <v>88</v>
       </c>
       <c r="D14" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="J14" s="6">
         <v>44745</v>
@@ -1163,27 +1163,27 @@
         <v>44765</v>
       </c>
       <c r="M14" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="P14" s="10" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>42</v>
+        <v>89</v>
       </c>
       <c r="D15" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="J15" s="8" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="K15" s="11">
         <v>44785</v>
@@ -1194,42 +1194,42 @@
     </row>
     <row r="16" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" t="s">
+        <v>90</v>
+      </c>
+      <c r="D16" t="s">
         <v>13</v>
       </c>
-      <c r="C16" t="s">
-        <v>43</v>
-      </c>
-      <c r="D16" t="s">
-        <v>17</v>
-      </c>
       <c r="J16" s="8" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="K16" s="11">
         <v>44785</v>
       </c>
       <c r="L16" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="P16" s="10" t="s">
         <v>20</v>
-      </c>
-      <c r="P16" s="10" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="5" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="B17" t="s">
         <v>6</v>
       </c>
       <c r="C17" t="s">
-        <v>45</v>
+        <v>91</v>
       </c>
       <c r="D17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J17" s="6">
         <v>44745</v>
@@ -1241,24 +1241,24 @@
         <v>44765</v>
       </c>
       <c r="M17" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="N17" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="B18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C18" t="s">
-        <v>48</v>
+        <v>92</v>
       </c>
       <c r="D18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J18" s="6">
         <v>44745</v>
@@ -1267,167 +1267,167 @@
         <v>44785</v>
       </c>
       <c r="L18" s="8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="B19" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C19" t="s">
-        <v>49</v>
+        <v>93</v>
       </c>
       <c r="D19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E19" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="H19" s="6">
         <v>44739</v>
       </c>
       <c r="J19" s="8" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="5" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="B20" t="s">
         <v>6</v>
       </c>
       <c r="C20" t="s">
-        <v>52</v>
+        <v>94</v>
       </c>
       <c r="D20" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="J20" s="8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="K20" s="10" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="B21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C21" t="s">
-        <v>54</v>
+        <v>95</v>
       </c>
       <c r="D21" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="J21" s="8" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="K21" s="11">
         <v>44785</v>
       </c>
       <c r="L21" s="10" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="B22" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C22" t="s">
-        <v>55</v>
+        <v>96</v>
       </c>
       <c r="D22" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="J22" s="8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="K22" s="10" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="5" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="B23" t="s">
         <v>6</v>
       </c>
       <c r="C23" t="s">
-        <v>57</v>
+        <v>97</v>
       </c>
       <c r="D23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J23" s="8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="K23" s="10" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="B24" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C24" t="s">
-        <v>58</v>
+        <v>98</v>
       </c>
       <c r="D24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E24" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="J24" s="8" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="B25" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C25" t="s">
-        <v>59</v>
+        <v>99</v>
       </c>
       <c r="D25" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J25" s="8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="5" t="s">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="B26" t="s">
         <v>6</v>
       </c>
       <c r="C26" t="s">
-        <v>61</v>
+        <v>100</v>
       </c>
       <c r="D26" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J26" s="8" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="K26" s="11">
         <v>44785</v>
@@ -1436,67 +1436,67 @@
         <v>44785</v>
       </c>
       <c r="P26" s="10" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="B27" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C27" t="s">
-        <v>62</v>
+        <v>101</v>
       </c>
       <c r="D27" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J27" s="8" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="M27" t="s">
-        <v>63</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="B28" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C28" t="s">
-        <v>64</v>
+        <v>102</v>
       </c>
       <c r="D28" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J28" s="8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="K28" s="13">
         <v>44732</v>
       </c>
       <c r="M28" t="s">
-        <v>65</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="5" t="s">
-        <v>66</v>
+        <v>39</v>
       </c>
       <c r="B29" t="s">
         <v>6</v>
       </c>
       <c r="C29" t="s">
-        <v>67</v>
+        <v>103</v>
       </c>
       <c r="D29" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E29" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G29" s="6">
         <v>44745</v>
@@ -1508,24 +1508,24 @@
         <v>44745</v>
       </c>
       <c r="M29" t="s">
-        <v>68</v>
+        <v>40</v>
       </c>
     </row>
     <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
-        <v>66</v>
+        <v>39</v>
       </c>
       <c r="B30" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C30" t="s">
-        <v>69</v>
+        <v>104</v>
       </c>
       <c r="D30" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E30" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G30" s="6">
         <v>44745</v>
@@ -1540,24 +1540,24 @@
         <v>44765</v>
       </c>
       <c r="M30" t="s">
-        <v>68</v>
+        <v>40</v>
       </c>
     </row>
     <row r="31" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
-        <v>66</v>
+        <v>39</v>
       </c>
       <c r="B31" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" t="s">
+        <v>105</v>
+      </c>
+      <c r="D31" t="s">
         <v>13</v>
       </c>
-      <c r="C31" t="s">
-        <v>70</v>
-      </c>
-      <c r="D31" t="s">
-        <v>17</v>
-      </c>
       <c r="E31" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="J31" s="11">
         <v>44785</v>
@@ -1565,16 +1565,16 @@
     </row>
     <row r="32" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="5" t="s">
-        <v>71</v>
+        <v>41</v>
       </c>
       <c r="B32" t="s">
         <v>6</v>
       </c>
       <c r="C32" t="s">
-        <v>72</v>
+        <v>106</v>
       </c>
       <c r="D32" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="J32" s="6">
         <v>44752</v>
@@ -1588,19 +1588,19 @@
     </row>
     <row r="33" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
-        <v>71</v>
+        <v>41</v>
       </c>
       <c r="B33" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C33" t="s">
-        <v>73</v>
+        <v>107</v>
       </c>
       <c r="D33" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="J33" s="8" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="K33" s="11">
         <v>44785</v>
@@ -1611,19 +1611,19 @@
     </row>
     <row r="34" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
-        <v>71</v>
+        <v>41</v>
       </c>
       <c r="B34" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C34" t="s">
-        <v>74</v>
+        <v>108</v>
       </c>
       <c r="D34" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="J34" s="8" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="K34" s="11">
         <v>44785</v>
@@ -1634,19 +1634,19 @@
     </row>
     <row r="35" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="5" t="s">
-        <v>75</v>
+        <v>42</v>
       </c>
       <c r="B35" t="s">
         <v>6</v>
       </c>
       <c r="C35" t="s">
-        <v>76</v>
+        <v>109</v>
       </c>
       <c r="D35" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E35" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G35" s="6"/>
       <c r="H35" s="6">
@@ -1656,96 +1656,96 @@
         <v>44745</v>
       </c>
       <c r="J35" s="8" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="M35" t="s">
-        <v>68</v>
+        <v>40</v>
       </c>
     </row>
     <row r="36" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
-        <v>75</v>
+        <v>42</v>
       </c>
       <c r="B36" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C36" t="s">
-        <v>77</v>
+        <v>110</v>
       </c>
       <c r="D36" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="J36" s="8" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="K36" s="11">
         <v>44785</v>
       </c>
       <c r="L36" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="M36" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="P36" s="10" t="s">
         <v>20</v>
-      </c>
-      <c r="M36" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="P36" s="10" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="37" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
-        <v>75</v>
+        <v>42</v>
       </c>
       <c r="B37" t="s">
+        <v>11</v>
+      </c>
+      <c r="C37" t="s">
+        <v>111</v>
+      </c>
+      <c r="D37" t="s">
         <v>13</v>
       </c>
-      <c r="C37" t="s">
-        <v>79</v>
-      </c>
-      <c r="D37" t="s">
-        <v>17</v>
-      </c>
       <c r="J37" s="8" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="K37" s="11">
         <v>44785</v>
       </c>
       <c r="L37" s="8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="38" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="5" t="s">
-        <v>80</v>
+        <v>44</v>
       </c>
       <c r="B38" t="s">
         <v>6</v>
       </c>
       <c r="C38" t="s">
-        <v>81</v>
+        <v>112</v>
       </c>
       <c r="D38" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J38" s="8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="39" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
-        <v>80</v>
+        <v>44</v>
       </c>
       <c r="B39" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C39" t="s">
-        <v>82</v>
+        <v>113</v>
       </c>
       <c r="D39" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J39" s="8" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="K39" s="11">
         <v>44785</v>
@@ -1753,19 +1753,19 @@
     </row>
     <row r="40" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
-        <v>80</v>
+        <v>44</v>
       </c>
       <c r="B40" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C40" t="s">
-        <v>83</v>
+        <v>114</v>
       </c>
       <c r="D40" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J40" s="8" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="K40" s="11">
         <v>44785</v>
@@ -1774,21 +1774,21 @@
         <v>44785</v>
       </c>
       <c r="N40" t="s">
-        <v>84</v>
+        <v>45</v>
       </c>
     </row>
     <row r="41" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="5" t="s">
-        <v>85</v>
+        <v>46</v>
       </c>
       <c r="B41" t="s">
         <v>6</v>
       </c>
       <c r="C41" t="s">
-        <v>86</v>
+        <v>115</v>
       </c>
       <c r="D41" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="J41" s="6">
         <v>44745</v>
@@ -1802,19 +1802,19 @@
     </row>
     <row r="42" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
-        <v>85</v>
+        <v>46</v>
       </c>
       <c r="B42" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C42" t="s">
-        <v>87</v>
+        <v>116</v>
       </c>
       <c r="D42" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="J42" s="8" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="K42" s="11">
         <v>44785</v>
@@ -1825,16 +1825,16 @@
     </row>
     <row r="43" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
-        <v>85</v>
+        <v>46</v>
       </c>
       <c r="B43" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C43" t="s">
-        <v>88</v>
+        <v>117</v>
       </c>
       <c r="D43" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="J43" s="6">
         <v>44745</v>
@@ -1848,16 +1848,16 @@
     </row>
     <row r="44" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="5" t="s">
-        <v>89</v>
+        <v>47</v>
       </c>
       <c r="B44" t="s">
         <v>6</v>
       </c>
       <c r="C44" t="s">
-        <v>90</v>
+        <v>118</v>
       </c>
       <c r="D44" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="J44" s="6">
         <v>44739</v>
@@ -1869,24 +1869,24 @@
         <v>44785</v>
       </c>
       <c r="M44" t="s">
-        <v>91</v>
+        <v>48</v>
       </c>
     </row>
     <row r="45" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
-        <v>89</v>
+        <v>47</v>
       </c>
       <c r="B45" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C45" t="s">
-        <v>92</v>
+        <v>119</v>
       </c>
       <c r="D45" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="J45" s="8" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="K45" s="11">
         <v>44785</v>
@@ -1897,19 +1897,19 @@
     </row>
     <row r="46" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
-        <v>89</v>
+        <v>47</v>
       </c>
       <c r="B46" t="s">
+        <v>11</v>
+      </c>
+      <c r="C46" t="s">
+        <v>120</v>
+      </c>
+      <c r="D46" t="s">
         <v>13</v>
       </c>
-      <c r="C46" t="s">
-        <v>93</v>
-      </c>
-      <c r="D46" t="s">
-        <v>17</v>
-      </c>
       <c r="J46" s="8" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="K46" s="11">
         <v>44785</v>
@@ -2176,95 +2176,95 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
-        <v>94</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>94</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="14" t="s">
-        <v>95</v>
+        <v>50</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>96</v>
+        <v>51</v>
       </c>
       <c r="C9" t="s">
-        <v>97</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="14" t="s">
-        <v>98</v>
+        <v>53</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>99</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="14" t="s">
-        <v>100</v>
+        <v>55</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>101</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="14" t="s">
-        <v>102</v>
+        <v>57</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>103</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="14" t="s">
-        <v>104</v>
+        <v>59</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>105</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="14" t="s">
-        <v>106</v>
+        <v>61</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>107</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="14" t="s">
-        <v>108</v>
+        <v>63</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>109</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
E corrects dates formatting
</commit_message>
<xml_diff>
--- a/data/phenology/groundtruthing_2022/FINAL_phenocam_groundtruthing_common_garden22_copy5.xlsx
+++ b/data/phenology/groundtruthing_2022/FINAL_phenocam_groundtruthing_common_garden22_copy5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericazaja/Desktop/Github_repos.tmp/GardenHub/data/phenology/groundtruthing_2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65EB8B22-04FA-A242-B05A-2C16F8E2F9FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ACE4EB7-9878-2B42-8FC8-6766BD471B4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="620" windowWidth="24640" windowHeight="15980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="118">
   <si>
     <t>Bed</t>
   </si>
@@ -53,9 +53,6 @@
     <t>B</t>
   </si>
   <si>
-    <t>31/07/22</t>
-  </si>
-  <si>
     <t>C</t>
   </si>
   <si>
@@ -66,12 +63,6 @@
   </si>
   <si>
     <t>female</t>
-  </si>
-  <si>
-    <t>17/07/22</t>
-  </si>
-  <si>
-    <t>17/08/22</t>
   </si>
   <si>
     <t>Catkin photos taken check with isla</t>
@@ -505,7 +496,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -528,6 +519,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -748,11 +741,11 @@
   </sheetPr>
   <dimension ref="A1:AA257"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="234" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E37" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="234" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="E23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C41" sqref="C41"/>
+      <selection pane="bottomRight" activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -774,37 +767,37 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>74</v>
       </c>
       <c r="M1" s="3" t="s">
         <v>2</v>
@@ -816,7 +809,7 @@
         <v>4</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
@@ -838,7 +831,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
@@ -865,7 +858,7 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>
@@ -880,8 +873,8 @@
         <v>44732</v>
       </c>
       <c r="I3" s="7"/>
-      <c r="J3" s="8" t="s">
-        <v>10</v>
+      <c r="J3" s="16">
+        <v>44773</v>
       </c>
     </row>
     <row r="4" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -889,10 +882,10 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
@@ -903,25 +896,25 @@
       <c r="G4" s="6">
         <v>44752</v>
       </c>
-      <c r="J4" s="8" t="s">
-        <v>10</v>
+      <c r="J4" s="16">
+        <v>44773</v>
       </c>
     </row>
     <row r="5" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
         <v>13</v>
-      </c>
-      <c r="E5" t="s">
-        <v>14</v>
       </c>
       <c r="H5" s="9">
         <v>44732</v>
@@ -929,31 +922,31 @@
       <c r="I5" s="9">
         <v>44745</v>
       </c>
-      <c r="J5" s="8" t="s">
+      <c r="J5" s="16">
+        <v>44759</v>
+      </c>
+      <c r="L5" s="17">
+        <v>44790</v>
+      </c>
+      <c r="M5" t="s">
+        <v>14</v>
+      </c>
+      <c r="N5" t="s">
         <v>15</v>
-      </c>
-      <c r="L5" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="M5" t="s">
-        <v>17</v>
-      </c>
-      <c r="N5" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J6" s="6">
         <v>44745</v>
@@ -965,42 +958,42 @@
         <v>44785</v>
       </c>
       <c r="M6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="P6" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D7" t="s">
         <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s">
-        <v>81</v>
-      </c>
-      <c r="D7" t="s">
-        <v>13</v>
       </c>
       <c r="J7" s="6">
         <v>44745</v>
       </c>
       <c r="K7" s="8"/>
       <c r="M7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D8" t="s">
         <v>7</v>
@@ -1008,25 +1001,25 @@
       <c r="J8" s="6">
         <v>44752</v>
       </c>
-      <c r="K8" s="10" t="s">
-        <v>16</v>
+      <c r="K8" s="17">
+        <v>44790</v>
       </c>
       <c r="L8" s="6">
         <v>44765</v>
       </c>
       <c r="M8" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D9" t="s">
         <v>7</v>
@@ -1041,21 +1034,21 @@
         <v>44785</v>
       </c>
       <c r="M9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="N9" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D10" t="s">
         <v>7</v>
@@ -1068,33 +1061,33 @@
         <v>44785</v>
       </c>
       <c r="M10" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="N10" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="O10" s="8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J11" s="6">
         <v>44752</v>
       </c>
-      <c r="K11" s="10" t="s">
-        <v>16</v>
+      <c r="K11" s="17">
+        <v>44790</v>
       </c>
       <c r="L11" s="11">
         <v>44785</v>
@@ -1102,19 +1095,19 @@
     </row>
     <row r="12" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B12" t="s">
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D12" t="s">
-        <v>13</v>
-      </c>
-      <c r="J12" s="8" t="s">
-        <v>15</v>
+        <v>12</v>
+      </c>
+      <c r="J12" s="16">
+        <v>44759</v>
       </c>
       <c r="K12" s="11">
         <v>44785</v>
@@ -1125,16 +1118,16 @@
     </row>
     <row r="13" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J13" s="6">
         <v>44745</v>
@@ -1142,16 +1135,16 @@
     </row>
     <row r="14" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B14" t="s">
         <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J14" s="6">
         <v>44745</v>
@@ -1163,27 +1156,27 @@
         <v>44765</v>
       </c>
       <c r="M14" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="P14" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B15" t="s">
         <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D15" t="s">
-        <v>13</v>
-      </c>
-      <c r="J15" s="8" t="s">
-        <v>15</v>
+        <v>12</v>
+      </c>
+      <c r="J15" s="16">
+        <v>44759</v>
       </c>
       <c r="K15" s="11">
         <v>44785</v>
@@ -1194,39 +1187,39 @@
     </row>
     <row r="16" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C16" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D16" t="s">
-        <v>13</v>
-      </c>
-      <c r="J16" s="8" t="s">
-        <v>15</v>
+        <v>12</v>
+      </c>
+      <c r="J16" s="16">
+        <v>44759</v>
       </c>
       <c r="K16" s="11">
         <v>44785</v>
       </c>
-      <c r="L16" s="10" t="s">
-        <v>16</v>
+      <c r="L16" s="17">
+        <v>44790</v>
       </c>
       <c r="P16" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B17" t="s">
         <v>6</v>
       </c>
       <c r="C17" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D17" t="s">
         <v>7</v>
@@ -1241,21 +1234,21 @@
         <v>44765</v>
       </c>
       <c r="M17" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="N17" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B18" t="s">
         <v>9</v>
       </c>
       <c r="C18" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D18" t="s">
         <v>7</v>
@@ -1266,168 +1259,168 @@
       <c r="K18" s="11">
         <v>44785</v>
       </c>
-      <c r="L18" s="8" t="s">
-        <v>10</v>
+      <c r="L18" s="16">
+        <v>44773</v>
       </c>
     </row>
     <row r="19" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C19" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D19" t="s">
         <v>7</v>
       </c>
       <c r="E19" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H19" s="6">
         <v>44739</v>
       </c>
-      <c r="J19" s="8" t="s">
-        <v>15</v>
+      <c r="J19" s="16">
+        <v>44759</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B20" t="s">
         <v>6</v>
       </c>
       <c r="C20" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D20" t="s">
-        <v>34</v>
-      </c>
-      <c r="J20" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="K20" s="10" t="s">
-        <v>16</v>
+        <v>31</v>
+      </c>
+      <c r="J20" s="16">
+        <v>44773</v>
+      </c>
+      <c r="K20" s="17">
+        <v>44790</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B21" t="s">
         <v>9</v>
       </c>
       <c r="C21" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D21" t="s">
-        <v>34</v>
-      </c>
-      <c r="J21" s="8" t="s">
-        <v>15</v>
+        <v>31</v>
+      </c>
+      <c r="J21" s="16">
+        <v>44759</v>
       </c>
       <c r="K21" s="11">
         <v>44785</v>
       </c>
-      <c r="L21" s="10" t="s">
-        <v>16</v>
+      <c r="L21" s="17">
+        <v>44790</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C22" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D22" t="s">
-        <v>34</v>
-      </c>
-      <c r="J22" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="K22" s="10" t="s">
-        <v>16</v>
+        <v>31</v>
+      </c>
+      <c r="J22" s="16">
+        <v>44773</v>
+      </c>
+      <c r="K22" s="17">
+        <v>44790</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B23" t="s">
         <v>6</v>
       </c>
       <c r="C23" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D23" t="s">
         <v>7</v>
       </c>
-      <c r="J23" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="K23" s="10" t="s">
-        <v>16</v>
+      <c r="J23" s="16">
+        <v>44773</v>
+      </c>
+      <c r="K23" s="17">
+        <v>44790</v>
       </c>
     </row>
     <row r="24" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B24" t="s">
         <v>9</v>
       </c>
       <c r="C24" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D24" t="s">
         <v>7</v>
       </c>
       <c r="E24" t="s">
-        <v>14</v>
-      </c>
-      <c r="J24" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
+      </c>
+      <c r="J24" s="16">
+        <v>44759</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C25" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D25" t="s">
         <v>7</v>
       </c>
-      <c r="J25" s="8" t="s">
-        <v>10</v>
+      <c r="J25" s="16">
+        <v>44773</v>
       </c>
     </row>
     <row r="26" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B26" t="s">
         <v>6</v>
       </c>
       <c r="C26" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D26" t="s">
         <v>7</v>
       </c>
-      <c r="J26" s="8" t="s">
-        <v>15</v>
+      <c r="J26" s="16">
+        <v>44759</v>
       </c>
       <c r="K26" s="11">
         <v>44785</v>
@@ -1436,64 +1429,64 @@
         <v>44785</v>
       </c>
       <c r="P26" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B27" t="s">
         <v>9</v>
       </c>
       <c r="C27" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D27" t="s">
         <v>7</v>
       </c>
-      <c r="J27" s="8" t="s">
-        <v>15</v>
+      <c r="J27" s="16">
+        <v>44759</v>
       </c>
       <c r="M27" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B28" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C28" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D28" t="s">
         <v>7</v>
       </c>
-      <c r="J28" s="8" t="s">
-        <v>10</v>
+      <c r="J28" s="16">
+        <v>44773</v>
       </c>
       <c r="K28" s="13">
         <v>44732</v>
       </c>
       <c r="M28" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B29" t="s">
         <v>6</v>
       </c>
       <c r="C29" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D29" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E29" t="s">
         <v>8</v>
@@ -1508,24 +1501,24 @@
         <v>44745</v>
       </c>
       <c r="M29" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B30" t="s">
         <v>9</v>
       </c>
       <c r="C30" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D30" t="s">
+        <v>12</v>
+      </c>
+      <c r="E30" t="s">
         <v>13</v>
-      </c>
-      <c r="E30" t="s">
-        <v>14</v>
       </c>
       <c r="G30" s="6">
         <v>44745</v>
@@ -1540,24 +1533,24 @@
         <v>44765</v>
       </c>
       <c r="M30" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="31" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B31" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C31" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D31" t="s">
+        <v>12</v>
+      </c>
+      <c r="E31" t="s">
         <v>13</v>
-      </c>
-      <c r="E31" t="s">
-        <v>14</v>
       </c>
       <c r="J31" s="11">
         <v>44785</v>
@@ -1565,16 +1558,16 @@
     </row>
     <row r="32" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B32" t="s">
         <v>6</v>
       </c>
       <c r="C32" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D32" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="J32" s="6">
         <v>44752</v>
@@ -1588,19 +1581,19 @@
     </row>
     <row r="33" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B33" t="s">
         <v>9</v>
       </c>
       <c r="C33" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D33" t="s">
-        <v>34</v>
-      </c>
-      <c r="J33" s="8" t="s">
-        <v>15</v>
+        <v>31</v>
+      </c>
+      <c r="J33" s="16">
+        <v>44759</v>
       </c>
       <c r="K33" s="11">
         <v>44785</v>
@@ -1611,19 +1604,19 @@
     </row>
     <row r="34" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B34" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C34" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D34" t="s">
-        <v>34</v>
-      </c>
-      <c r="J34" s="8" t="s">
-        <v>15</v>
+        <v>31</v>
+      </c>
+      <c r="J34" s="16">
+        <v>44759</v>
       </c>
       <c r="K34" s="11">
         <v>44785</v>
@@ -1634,19 +1627,19 @@
     </row>
     <row r="35" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B35" t="s">
         <v>6</v>
       </c>
       <c r="C35" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D35" t="s">
+        <v>12</v>
+      </c>
+      <c r="E35" t="s">
         <v>13</v>
-      </c>
-      <c r="E35" t="s">
-        <v>14</v>
       </c>
       <c r="G35" s="6"/>
       <c r="H35" s="6">
@@ -1655,97 +1648,97 @@
       <c r="I35" s="6">
         <v>44745</v>
       </c>
-      <c r="J35" s="8" t="s">
-        <v>15</v>
+      <c r="J35" s="16">
+        <v>44759</v>
       </c>
       <c r="M35" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="36" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B36" t="s">
         <v>9</v>
       </c>
       <c r="C36" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D36" t="s">
-        <v>13</v>
-      </c>
-      <c r="J36" s="8" t="s">
-        <v>15</v>
+        <v>12</v>
+      </c>
+      <c r="J36" s="16">
+        <v>44759</v>
       </c>
       <c r="K36" s="11">
         <v>44785</v>
       </c>
-      <c r="L36" s="10" t="s">
-        <v>16</v>
+      <c r="L36" s="17">
+        <v>44790</v>
       </c>
       <c r="M36" s="8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="P36" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="37" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B37" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C37" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D37" t="s">
-        <v>13</v>
-      </c>
-      <c r="J37" s="8" t="s">
-        <v>15</v>
+        <v>12</v>
+      </c>
+      <c r="J37" s="16">
+        <v>44759</v>
       </c>
       <c r="K37" s="11">
         <v>44785</v>
       </c>
-      <c r="L37" s="8" t="s">
-        <v>10</v>
+      <c r="L37" s="16">
+        <v>44773</v>
       </c>
     </row>
     <row r="38" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B38" t="s">
         <v>6</v>
       </c>
       <c r="C38" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D38" t="s">
         <v>7</v>
       </c>
-      <c r="J38" s="8" t="s">
-        <v>10</v>
+      <c r="J38" s="16">
+        <v>44773</v>
       </c>
     </row>
     <row r="39" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B39" t="s">
         <v>9</v>
       </c>
       <c r="C39" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D39" t="s">
         <v>7</v>
       </c>
-      <c r="J39" s="8" t="s">
-        <v>15</v>
+      <c r="J39" s="16">
+        <v>44759</v>
       </c>
       <c r="K39" s="11">
         <v>44785</v>
@@ -1753,19 +1746,19 @@
     </row>
     <row r="40" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B40" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C40" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D40" t="s">
         <v>7</v>
       </c>
-      <c r="J40" s="8" t="s">
-        <v>15</v>
+      <c r="J40" s="16">
+        <v>44759</v>
       </c>
       <c r="K40" s="11">
         <v>44785</v>
@@ -1774,21 +1767,21 @@
         <v>44785</v>
       </c>
       <c r="N40" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="41" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B41" t="s">
         <v>6</v>
       </c>
       <c r="C41" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D41" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="J41" s="6">
         <v>44745</v>
@@ -1802,19 +1795,19 @@
     </row>
     <row r="42" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B42" t="s">
         <v>9</v>
       </c>
       <c r="C42" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D42" t="s">
-        <v>34</v>
-      </c>
-      <c r="J42" s="8" t="s">
-        <v>15</v>
+        <v>31</v>
+      </c>
+      <c r="J42" s="16">
+        <v>44759</v>
       </c>
       <c r="K42" s="11">
         <v>44785</v>
@@ -1825,16 +1818,16 @@
     </row>
     <row r="43" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B43" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C43" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D43" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="J43" s="6">
         <v>44745</v>
@@ -1848,16 +1841,16 @@
     </row>
     <row r="44" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B44" t="s">
         <v>6</v>
       </c>
       <c r="C44" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D44" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="J44" s="6">
         <v>44739</v>
@@ -1869,24 +1862,24 @@
         <v>44785</v>
       </c>
       <c r="M44" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="45" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B45" t="s">
         <v>9</v>
       </c>
       <c r="C45" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D45" t="s">
-        <v>13</v>
-      </c>
-      <c r="J45" s="8" t="s">
-        <v>15</v>
+        <v>12</v>
+      </c>
+      <c r="J45" s="16">
+        <v>44759</v>
       </c>
       <c r="K45" s="11">
         <v>44785</v>
@@ -1897,19 +1890,19 @@
     </row>
     <row r="46" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C46" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D46" t="s">
-        <v>13</v>
-      </c>
-      <c r="J46" s="8" t="s">
-        <v>15</v>
+        <v>12</v>
+      </c>
+      <c r="J46" s="16">
+        <v>44759</v>
       </c>
       <c r="K46" s="11">
         <v>44785</v>
@@ -2176,10 +2169,10 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2189,7 +2182,7 @@
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2198,73 +2191,73 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="14" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="14" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="14" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="14" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="14" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="14" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="14" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
E puts data into long format
</commit_message>
<xml_diff>
--- a/data/phenology/groundtruthing_2022/FINAL_phenocam_groundtruthing_common_garden22_copy5.xlsx
+++ b/data/phenology/groundtruthing_2022/FINAL_phenocam_groundtruthing_common_garden22_copy5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericazaja/Desktop/Github_repos.tmp/GardenHub/data/phenology/groundtruthing_2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ACE4EB7-9878-2B42-8FC8-6766BD471B4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E5F1A61-7C79-8542-9019-44DC8483029C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="620" windowWidth="24640" windowHeight="15980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="121">
   <si>
     <t>Bed</t>
   </si>
@@ -375,6 +375,15 @@
   </si>
   <si>
     <t>H18Sr27</t>
+  </si>
+  <si>
+    <t>Salix pulchra</t>
+  </si>
+  <si>
+    <t>Salix richardsonii</t>
+  </si>
+  <si>
+    <t>Salix arctica</t>
   </si>
 </sst>
 </file>
@@ -742,10 +751,10 @@
   <dimension ref="A1:AA257"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="234" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="I26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L12" sqref="L12"/>
+      <selection pane="bottomRight" activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -834,7 +843,7 @@
         <v>73</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>118</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
@@ -861,7 +870,7 @@
         <v>74</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>118</v>
       </c>
       <c r="E3" t="s">
         <v>8</v>
@@ -888,7 +897,7 @@
         <v>75</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>118</v>
       </c>
       <c r="F4" s="6">
         <v>44752</v>
@@ -911,7 +920,7 @@
         <v>76</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>119</v>
       </c>
       <c r="E5" t="s">
         <v>13</v>
@@ -946,7 +955,7 @@
         <v>77</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
+        <v>119</v>
       </c>
       <c r="J6" s="6">
         <v>44745</v>
@@ -975,7 +984,7 @@
         <v>78</v>
       </c>
       <c r="D7" t="s">
-        <v>12</v>
+        <v>119</v>
       </c>
       <c r="J7" s="6">
         <v>44745</v>
@@ -996,7 +1005,7 @@
         <v>79</v>
       </c>
       <c r="D8" t="s">
-        <v>7</v>
+        <v>118</v>
       </c>
       <c r="J8" s="6">
         <v>44752</v>
@@ -1022,7 +1031,7 @@
         <v>80</v>
       </c>
       <c r="D9" t="s">
-        <v>7</v>
+        <v>118</v>
       </c>
       <c r="J9" s="6">
         <v>44745</v>
@@ -1051,7 +1060,7 @@
         <v>81</v>
       </c>
       <c r="D10" t="s">
-        <v>7</v>
+        <v>118</v>
       </c>
       <c r="J10" s="6">
         <v>44752</v>
@@ -1081,7 +1090,7 @@
         <v>82</v>
       </c>
       <c r="D11" t="s">
-        <v>12</v>
+        <v>119</v>
       </c>
       <c r="J11" s="6">
         <v>44752</v>
@@ -1104,7 +1113,7 @@
         <v>83</v>
       </c>
       <c r="D12" t="s">
-        <v>12</v>
+        <v>119</v>
       </c>
       <c r="J12" s="16">
         <v>44759</v>
@@ -1127,7 +1136,7 @@
         <v>84</v>
       </c>
       <c r="D13" t="s">
-        <v>12</v>
+        <v>119</v>
       </c>
       <c r="J13" s="6">
         <v>44745</v>
@@ -1144,7 +1153,7 @@
         <v>85</v>
       </c>
       <c r="D14" t="s">
-        <v>12</v>
+        <v>119</v>
       </c>
       <c r="J14" s="6">
         <v>44745</v>
@@ -1173,7 +1182,7 @@
         <v>86</v>
       </c>
       <c r="D15" t="s">
-        <v>12</v>
+        <v>119</v>
       </c>
       <c r="J15" s="16">
         <v>44759</v>
@@ -1196,7 +1205,7 @@
         <v>87</v>
       </c>
       <c r="D16" t="s">
-        <v>12</v>
+        <v>119</v>
       </c>
       <c r="J16" s="16">
         <v>44759</v>
@@ -1222,7 +1231,7 @@
         <v>88</v>
       </c>
       <c r="D17" t="s">
-        <v>7</v>
+        <v>118</v>
       </c>
       <c r="J17" s="6">
         <v>44745</v>
@@ -1251,7 +1260,7 @@
         <v>89</v>
       </c>
       <c r="D18" t="s">
-        <v>7</v>
+        <v>118</v>
       </c>
       <c r="J18" s="6">
         <v>44745</v>
@@ -1274,7 +1283,7 @@
         <v>90</v>
       </c>
       <c r="D19" t="s">
-        <v>7</v>
+        <v>118</v>
       </c>
       <c r="E19" t="s">
         <v>29</v>
@@ -1297,7 +1306,7 @@
         <v>91</v>
       </c>
       <c r="D20" t="s">
-        <v>31</v>
+        <v>120</v>
       </c>
       <c r="J20" s="16">
         <v>44773</v>
@@ -1317,7 +1326,7 @@
         <v>92</v>
       </c>
       <c r="D21" t="s">
-        <v>31</v>
+        <v>120</v>
       </c>
       <c r="J21" s="16">
         <v>44759</v>
@@ -1340,7 +1349,7 @@
         <v>93</v>
       </c>
       <c r="D22" t="s">
-        <v>31</v>
+        <v>120</v>
       </c>
       <c r="J22" s="16">
         <v>44773</v>
@@ -1360,7 +1369,7 @@
         <v>94</v>
       </c>
       <c r="D23" t="s">
-        <v>7</v>
+        <v>118</v>
       </c>
       <c r="J23" s="16">
         <v>44773</v>
@@ -1380,7 +1389,7 @@
         <v>95</v>
       </c>
       <c r="D24" t="s">
-        <v>7</v>
+        <v>118</v>
       </c>
       <c r="E24" t="s">
         <v>13</v>
@@ -1400,7 +1409,7 @@
         <v>96</v>
       </c>
       <c r="D25" t="s">
-        <v>7</v>
+        <v>118</v>
       </c>
       <c r="J25" s="16">
         <v>44773</v>
@@ -1417,7 +1426,7 @@
         <v>97</v>
       </c>
       <c r="D26" t="s">
-        <v>7</v>
+        <v>118</v>
       </c>
       <c r="J26" s="16">
         <v>44759</v>
@@ -1443,7 +1452,7 @@
         <v>98</v>
       </c>
       <c r="D27" t="s">
-        <v>7</v>
+        <v>118</v>
       </c>
       <c r="J27" s="16">
         <v>44759</v>
@@ -1463,7 +1472,7 @@
         <v>99</v>
       </c>
       <c r="D28" t="s">
-        <v>7</v>
+        <v>118</v>
       </c>
       <c r="J28" s="16">
         <v>44773</v>
@@ -1486,7 +1495,7 @@
         <v>100</v>
       </c>
       <c r="D29" t="s">
-        <v>12</v>
+        <v>119</v>
       </c>
       <c r="E29" t="s">
         <v>8</v>
@@ -1515,7 +1524,7 @@
         <v>101</v>
       </c>
       <c r="D30" t="s">
-        <v>12</v>
+        <v>119</v>
       </c>
       <c r="E30" t="s">
         <v>13</v>
@@ -1547,7 +1556,7 @@
         <v>102</v>
       </c>
       <c r="D31" t="s">
-        <v>12</v>
+        <v>119</v>
       </c>
       <c r="E31" t="s">
         <v>13</v>
@@ -1567,7 +1576,7 @@
         <v>103</v>
       </c>
       <c r="D32" t="s">
-        <v>31</v>
+        <v>120</v>
       </c>
       <c r="J32" s="6">
         <v>44752</v>
@@ -1590,7 +1599,7 @@
         <v>104</v>
       </c>
       <c r="D33" t="s">
-        <v>31</v>
+        <v>120</v>
       </c>
       <c r="J33" s="16">
         <v>44759</v>
@@ -1613,7 +1622,7 @@
         <v>105</v>
       </c>
       <c r="D34" t="s">
-        <v>31</v>
+        <v>120</v>
       </c>
       <c r="J34" s="16">
         <v>44759</v>
@@ -1636,7 +1645,7 @@
         <v>106</v>
       </c>
       <c r="D35" t="s">
-        <v>12</v>
+        <v>119</v>
       </c>
       <c r="E35" t="s">
         <v>13</v>
@@ -1666,7 +1675,7 @@
         <v>107</v>
       </c>
       <c r="D36" t="s">
-        <v>12</v>
+        <v>119</v>
       </c>
       <c r="J36" s="16">
         <v>44759</v>
@@ -1695,7 +1704,7 @@
         <v>108</v>
       </c>
       <c r="D37" t="s">
-        <v>12</v>
+        <v>119</v>
       </c>
       <c r="J37" s="16">
         <v>44759</v>
@@ -1718,7 +1727,7 @@
         <v>109</v>
       </c>
       <c r="D38" t="s">
-        <v>7</v>
+        <v>118</v>
       </c>
       <c r="J38" s="16">
         <v>44773</v>
@@ -1735,7 +1744,7 @@
         <v>110</v>
       </c>
       <c r="D39" t="s">
-        <v>7</v>
+        <v>118</v>
       </c>
       <c r="J39" s="16">
         <v>44759</v>
@@ -1755,7 +1764,7 @@
         <v>111</v>
       </c>
       <c r="D40" t="s">
-        <v>7</v>
+        <v>118</v>
       </c>
       <c r="J40" s="16">
         <v>44759</v>
@@ -1781,7 +1790,7 @@
         <v>112</v>
       </c>
       <c r="D41" t="s">
-        <v>31</v>
+        <v>120</v>
       </c>
       <c r="J41" s="6">
         <v>44745</v>
@@ -1804,7 +1813,7 @@
         <v>113</v>
       </c>
       <c r="D42" t="s">
-        <v>31</v>
+        <v>120</v>
       </c>
       <c r="J42" s="16">
         <v>44759</v>
@@ -1827,7 +1836,7 @@
         <v>114</v>
       </c>
       <c r="D43" t="s">
-        <v>31</v>
+        <v>120</v>
       </c>
       <c r="J43" s="6">
         <v>44745</v>
@@ -1850,7 +1859,7 @@
         <v>115</v>
       </c>
       <c r="D44" t="s">
-        <v>31</v>
+        <v>120</v>
       </c>
       <c r="J44" s="6">
         <v>44739</v>
@@ -1876,7 +1885,7 @@
         <v>116</v>
       </c>
       <c r="D45" t="s">
-        <v>12</v>
+        <v>119</v>
       </c>
       <c r="J45" s="16">
         <v>44759</v>
@@ -1899,7 +1908,7 @@
         <v>117</v>
       </c>
       <c r="D46" t="s">
-        <v>12</v>
+        <v>119</v>
       </c>
       <c r="J46" s="16">
         <v>44759</v>

</xml_diff>